<commit_message>
tabla dns completa (con valores no reales)
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
+++ b/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="159">
   <si>
     <t>R1</t>
   </si>
@@ -293,12 +293,6 @@
     <t>GRE</t>
   </si>
   <si>
-    <t>Marin - 10.47.1.128/26 - (.giant.elcalafate.stacruz.dc.fi.uba.ar)</t>
-  </si>
-  <si>
-    <t>Ghost - 10.19.3.144/29 - (.kona.elcalafate.stacruz.dc.fi.uba.ar)</t>
-  </si>
-  <si>
     <t>Enlaces</t>
   </si>
   <si>
@@ -437,7 +431,73 @@
     <t>Conor - 10.19.3.8/30 - (.conor.stacruz.dc.fi.uba.ar)</t>
   </si>
   <si>
-    <t>..</t>
+    <t>.9</t>
+  </si>
+  <si>
+    <t>.10</t>
+  </si>
+  <si>
+    <t>.13</t>
+  </si>
+  <si>
+    <t>.14</t>
+  </si>
+  <si>
+    <t>Ghost - 10.19.3.152/30 - (.ghost.stacruz.dc.fi.uba.ar)</t>
+  </si>
+  <si>
+    <t>.153</t>
+  </si>
+  <si>
+    <t>.154</t>
+  </si>
+  <si>
+    <t>r1.bianchi1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r13.bianchi2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r1.couler1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r12.couler2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r12.yeti1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r13.yeti2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r5.conor1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r8.conor2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>Marin - 10.19.3.12/30 - (.marin.stacruz.dc.fi.uba.ar)</t>
+  </si>
+  <si>
+    <t>r8.marin1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r16.marin2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r5.ghost1.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r16.ghost2.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r2.orbea1.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r16.orbea2.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -527,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -721,19 +781,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -743,7 +790,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -856,6 +903,57 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,15 +963,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -882,51 +971,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1236,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1258,24 +1302,26 @@
       <c r="C1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="14" t="s">
+        <v>158</v>
+      </c>
       <c r="E1" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1285,12 +1331,12 @@
       <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="52" t="s">
-        <v>100</v>
+      <c r="E3" s="42" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1300,12 +1346,12 @@
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="52" t="s">
-        <v>101</v>
+      <c r="E4" s="42" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1315,12 +1361,12 @@
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="52" t="s">
-        <v>102</v>
+      <c r="E5" s="42" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1330,12 +1376,12 @@
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="52" t="s">
-        <v>103</v>
+      <c r="E6" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
@@ -1346,11 +1392,11 @@
         <v>42</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="17" t="s">
         <v>56</v>
       </c>
@@ -1361,20 +1407,20 @@
         <v>48</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
     </row>
     <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="15" t="s">
         <v>2</v>
       </c>
@@ -1384,12 +1430,12 @@
       <c r="D10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="51" t="s">
-        <v>97</v>
+      <c r="E10" s="41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="11" t="s">
         <v>3</v>
       </c>
@@ -1399,12 +1445,12 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="51" t="s">
-        <v>98</v>
+      <c r="E11" s="41" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
@@ -1414,12 +1460,12 @@
       <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="51" t="s">
-        <v>99</v>
+      <c r="E12" s="41" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="17" t="s">
         <v>59</v>
       </c>
@@ -1430,22 +1476,22 @@
         <v>9</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
@@ -1455,12 +1501,12 @@
       <c r="D15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="51" t="s">
-        <v>104</v>
+      <c r="E15" s="41" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
@@ -1470,12 +1516,12 @@
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="51" t="s">
-        <v>105</v>
+      <c r="E16" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="22" t="s">
         <v>61</v>
       </c>
@@ -1486,20 +1532,20 @@
         <v>40</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="44" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
     </row>
     <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
@@ -1509,12 +1555,12 @@
       <c r="D19" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="51" t="s">
-        <v>107</v>
+      <c r="E19" s="41" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
@@ -1524,12 +1570,12 @@
       <c r="D20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="51" t="s">
-        <v>108</v>
+      <c r="E20" s="41" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="11" t="s">
         <v>30</v>
       </c>
@@ -1539,12 +1585,12 @@
       <c r="D21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="51" t="s">
-        <v>109</v>
+      <c r="E21" s="41" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="22" t="s">
         <v>22</v>
       </c>
@@ -1554,21 +1600,21 @@
       <c r="D22" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="51" t="s">
-        <v>110</v>
+      <c r="E22" s="41" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="38" t="s">
+      <c r="A23" s="53"/>
+      <c r="B23" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="28" t="s">
         <v>28</v>
       </c>
@@ -1578,12 +1624,12 @@
       <c r="D24" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="53" t="s">
-        <v>115</v>
+      <c r="E24" s="43" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="11" t="s">
         <v>22</v>
       </c>
@@ -1593,12 +1639,12 @@
       <c r="D25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="51" t="s">
-        <v>112</v>
+      <c r="E25" s="41" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
@@ -1608,12 +1654,12 @@
       <c r="D26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="51" t="s">
-        <v>113</v>
+      <c r="E26" s="41" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="11" t="s">
         <v>24</v>
       </c>
@@ -1623,12 +1669,12 @@
       <c r="D27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="51" t="s">
-        <v>114</v>
+      <c r="E27" s="41" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="30" t="s">
         <v>66</v>
       </c>
@@ -1639,20 +1685,20 @@
         <v>68</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
-      <c r="B29" s="38" t="s">
+      <c r="A29" s="53"/>
+      <c r="B29" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="40"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
     </row>
     <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
@@ -1662,12 +1708,12 @@
       <c r="D30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="51" t="s">
-        <v>116</v>
+      <c r="E30" s="41" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="11" t="s">
         <v>22</v>
       </c>
@@ -1677,12 +1723,12 @@
       <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="51" t="s">
-        <v>117</v>
+      <c r="E31" s="41" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="22" t="s">
         <v>23</v>
       </c>
@@ -1692,23 +1738,23 @@
       <c r="D32" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="51" t="s">
-        <v>118</v>
+      <c r="E32" s="41" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="40"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="57"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="33" t="s">
         <v>37</v>
       </c>
@@ -1719,11 +1765,11 @@
         <v>39</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="11" t="s">
         <v>43</v>
       </c>
@@ -1734,11 +1780,11 @@
         <v>45</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="11" t="s">
         <v>44</v>
       </c>
@@ -1748,36 +1794,36 @@
       <c r="D36" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="54" t="s">
-        <v>120</v>
+      <c r="E36" s="44" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>119</v>
+      <c r="E37" s="41" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="38" t="s">
+      <c r="A38" s="53"/>
+      <c r="B38" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="57"/>
     </row>
     <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="33" t="s">
         <v>37</v>
       </c>
@@ -1788,11 +1834,11 @@
         <v>39</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="10" t="s">
         <v>47</v>
       </c>
@@ -1803,11 +1849,11 @@
         <v>75</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="42"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="22" t="s">
         <v>30</v>
       </c>
@@ -1818,20 +1864,20 @@
         <v>35</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="42"/>
-      <c r="B42" s="38" t="s">
+      <c r="A42" s="53"/>
+      <c r="B42" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="57"/>
     </row>
     <row r="43" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="42"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="35" t="s">
         <v>44</v>
       </c>
@@ -1842,20 +1888,20 @@
         <v>46</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="42"/>
-      <c r="B44" s="38" t="s">
+      <c r="A44" s="53"/>
+      <c r="B44" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="57"/>
     </row>
     <row r="45" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="43"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="15" t="s">
         <v>44</v>
       </c>
@@ -1863,73 +1909,79 @@
         <v>74</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40"/>
+      <c r="B46" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="57"/>
     </row>
     <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="9"/>
+      <c r="E47" s="9" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="42"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="55" t="s">
+      <c r="D48" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="53"/>
+      <c r="B49" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="D48" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="19"/>
-    </row>
-    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="42"/>
-      <c r="B49" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="57"/>
     </row>
     <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
-      <c r="B50" s="56" t="s">
+      <c r="A50" s="53"/>
+      <c r="B50" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="57" t="s">
+      <c r="C50" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="D50" s="57" t="s">
+      <c r="D50" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E50" s="58"/>
+      <c r="E50" s="48" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="42"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="22" t="s">
         <v>24</v>
       </c>
@@ -1939,133 +1991,181 @@
       <c r="D51" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="27"/>
+      <c r="E51" s="48" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
+      <c r="A52" s="53"/>
+      <c r="B52" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="57"/>
     </row>
     <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="27"/>
+      <c r="E53" s="27" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="42"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C54" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="57"/>
+    </row>
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="53"/>
+      <c r="B56" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D54" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" s="37"/>
-    </row>
-    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="38" t="s">
+      <c r="D56" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="53"/>
+      <c r="B57" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="40"/>
-    </row>
-    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="42"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="18"/>
       <c r="D57" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="53"/>
+      <c r="B58" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="57"/>
+    </row>
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="53"/>
+      <c r="B60" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="42"/>
-      <c r="B58" s="38" t="s">
+      <c r="E60" s="42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="53"/>
+      <c r="B61" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="57"/>
+    </row>
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="53"/>
+      <c r="B62" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="53"/>
+      <c r="B63" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D63" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="40"/>
-    </row>
-    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="42"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="27"/>
-    </row>
-    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="42"/>
-      <c r="B61" s="38" t="s">
+      <c r="B64" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="40"/>
-    </row>
-    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="42"/>
-      <c r="B62" s="22"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="27"/>
-    </row>
-    <row r="63" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="42"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="37"/>
-    </row>
-    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="40"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="57"/>
     </row>
     <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
+      <c r="A65" s="53"/>
       <c r="B65" s="11" t="s">
         <v>1</v>
       </c>
@@ -2075,34 +2175,27 @@
       <c r="D65" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E65" s="47"/>
+      <c r="E65" s="38" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="43"/>
-      <c r="B66" s="48" t="s">
+      <c r="A66" s="54"/>
+      <c r="B66" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="61" t="s">
+      <c r="C66" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="49" t="s">
+      <c r="D66" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E66" s="50"/>
+      <c r="E66" s="38" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="A46:A54"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B23:E23"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A33:A45"/>
@@ -2115,6 +2208,17 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B33:E33"/>
+    <mergeCell ref="A46:A54"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1" display="ftp.baires.dc.fi.uba.ar"/>

</xml_diff>

<commit_message>
Cambios en los .rev y tabla de dns (hasta el momento sede rio gallegos y el calafate)
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
+++ b/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FIUBA-tps\distrib\tp-distribuidos-grupo3\ tp-distribuidos-grupo3\DNS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="11730" windowHeight="5580"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="168">
   <si>
     <t>R1</t>
   </si>
@@ -209,9 +204,6 @@
     <t>HostB</t>
   </si>
   <si>
-    <t>10.19.3.32</t>
-  </si>
-  <si>
     <t>.33</t>
   </si>
   <si>
@@ -299,24 +291,12 @@
     <t>Raleigh - 10.47.2.0/24 - (.orbea.elcalafate.stacruz.dc.fi.uba.ar)</t>
   </si>
   <si>
-    <t>ns1.trek7.rioturbio.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
     <t>hosta.trek6.rioturbio.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
     <t>webserver.specialized1.rioturbio.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
-    <t>r3.specialized3.rioturbio.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
-    <t>r4.specialized4.rioturbio.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
-    <t>r5.specialized5.rioturbio.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
     <t>r1.trek1.rioturbio.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
@@ -350,9 +330,6 @@
     <t>r10.lapierre4.riogallegos.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
-    <t>ns2.bh1.riogallegos.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
     <t>r10.bh3.riogallegos.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
@@ -362,9 +339,6 @@
     <t>r12.bh5.riogallegos.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
-    <t>ftp.bh2.riogallegos.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
     <t>r9.cannondale1.riogallegos.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
@@ -498,6 +472,54 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>r3.specialized1.rioturbio.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r5.specialized3.rioturbio.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ns1.trek.rioturbio.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r5.specialized2.rioturbio.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>10.19.3.35</t>
+  </si>
+  <si>
+    <t>ns2.bh.riogallegos.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>ftpserver.bh2.riogallegos.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>Scott - 10.19.3.96/27 - (.scott.elcalafate.stacruz.dc.fi.uba.ar)</t>
+  </si>
+  <si>
+    <t>HostC</t>
+  </si>
+  <si>
+    <t>10.47.1.97</t>
+  </si>
+  <si>
+    <t>.98</t>
+  </si>
+  <si>
+    <t>.99</t>
+  </si>
+  <si>
+    <t>hostc</t>
+  </si>
+  <si>
+    <t>r13.scott1.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r14.scott2.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>hostc.scott3.elcalafate.stacruz.dc.fi.uba.ar</t>
   </si>
 </sst>
 </file>
@@ -945,6 +967,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -954,15 +985,6 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,8 +996,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -992,7 +1014,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1034,7 +1056,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1069,7 +1091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1278,19 +1300,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1303,25 +1325,25 @@
         <v>53</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
+      <c r="B2" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1332,11 +1354,11 @@
         <v>10</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1347,11 +1369,11 @@
         <v>11</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1362,11 +1384,11 @@
         <v>12</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1377,11 +1399,11 @@
         <v>13</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
@@ -1392,11 +1414,11 @@
         <v>42</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="17" t="s">
         <v>56</v>
       </c>
@@ -1407,20 +1429,20 @@
         <v>48</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
     </row>
     <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="15" t="s">
         <v>2</v>
       </c>
@@ -1431,11 +1453,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="11" t="s">
         <v>3</v>
       </c>
@@ -1446,11 +1468,11 @@
         <v>13</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
@@ -1461,11 +1483,11 @@
         <v>21</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="17" t="s">
         <v>59</v>
       </c>
@@ -1476,76 +1498,76 @@
         <v>9</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="B14" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
     </row>
     <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="22" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="53"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
       <c r="E18" s="60"/>
     </row>
     <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
@@ -1556,11 +1578,11 @@
         <v>18</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
@@ -1571,11 +1593,11 @@
         <v>19</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="11" t="s">
         <v>30</v>
       </c>
@@ -1586,11 +1608,11 @@
         <v>35</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="22" t="s">
         <v>22</v>
       </c>
@@ -1601,35 +1623,35 @@
         <v>25</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="11" t="s">
         <v>22</v>
       </c>
@@ -1640,11 +1662,11 @@
         <v>25</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
@@ -1655,11 +1677,11 @@
         <v>26</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="11" t="s">
         <v>24</v>
       </c>
@@ -1670,106 +1692,106 @@
         <v>27</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="53"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
-      <c r="B29" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
     </row>
     <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
+      <c r="B33" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="54"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="11" t="s">
         <v>43</v>
       </c>
@@ -1780,11 +1802,11 @@
         <v>45</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="11" t="s">
         <v>44</v>
       </c>
@@ -1795,11 +1817,11 @@
         <v>46</v>
       </c>
       <c r="E36" s="44" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="53"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="22" t="s">
         <v>36</v>
       </c>
@@ -1810,50 +1832,50 @@
         <v>38</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="53"/>
-      <c r="B38" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="57"/>
+      <c r="A38" s="56"/>
+      <c r="B38" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="54"/>
     </row>
     <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="53"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="53"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="22" t="s">
         <v>30</v>
       </c>
@@ -1864,341 +1886,407 @@
         <v>35</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="53"/>
-      <c r="B42" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="57"/>
+      <c r="A42" s="56"/>
+      <c r="B42" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
     </row>
     <row r="43" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="53"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="36" t="s">
         <v>46</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="53"/>
-      <c r="B44" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="57"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
     </row>
     <row r="45" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="54"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>46</v>
       </c>
       <c r="E45" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="56"/>
+      <c r="B46" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="56"/>
+      <c r="B47" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="56"/>
+      <c r="B48" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="57"/>
+      <c r="B49" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="54"/>
+    </row>
+    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="56"/>
+      <c r="B51" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="56"/>
+      <c r="B52" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="56"/>
+      <c r="B53" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="54"/>
+    </row>
+    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="56"/>
+      <c r="B54" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="56"/>
+      <c r="B55" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="56"/>
+      <c r="B56" s="52" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52" t="s">
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54"/>
+    </row>
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="56"/>
+      <c r="B57" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="56"/>
+      <c r="B58" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="57"/>
-    </row>
-    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="B59" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="9" t="s">
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="54"/>
+    </row>
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="56"/>
+      <c r="B60" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="56"/>
+      <c r="B61" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="53"/>
-      <c r="B48" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="E48" s="9" t="s">
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="56"/>
+      <c r="B62" s="52" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="53"/>
-      <c r="B49" s="55" t="s">
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="54"/>
+    </row>
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="56"/>
+      <c r="B63" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="57"/>
-    </row>
-    <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
-      <c r="B50" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="D50" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="48" t="s">
+      <c r="D63" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="53"/>
-      <c r="B51" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="48" t="s">
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="56"/>
+      <c r="B64" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="53"/>
-      <c r="B52" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="57"/>
-    </row>
-    <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="53"/>
-      <c r="B53" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="25" t="s">
+    <row r="65" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="56"/>
+      <c r="B65" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="27" t="s">
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="54"/>
+    </row>
+    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="56"/>
+      <c r="B66" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="53"/>
-      <c r="B54" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="E54" s="27" t="s">
+    <row r="67" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="56"/>
+      <c r="B67" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="52" t="s">
+    <row r="68" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="57"/>
-    </row>
-    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="53"/>
-      <c r="B56" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56" s="9" t="s">
+      <c r="B68" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="53"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="54"/>
+    </row>
+    <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="56"/>
+      <c r="B69" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="38" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="53"/>
-      <c r="B57" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="9" t="s">
+    <row r="70" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="57"/>
+      <c r="B70" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="38" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="53"/>
-      <c r="B58" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="57"/>
-    </row>
-    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53"/>
-      <c r="B59" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="50" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="42" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="53"/>
-      <c r="B60" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="53"/>
-      <c r="B61" s="55" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="57"/>
-    </row>
-    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="53"/>
-      <c r="B62" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="53"/>
-      <c r="B63" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C63" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D63" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E63" s="27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="57"/>
-    </row>
-    <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="53"/>
-      <c r="B65" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
-      <c r="B66" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="38" t="s">
-        <v>157</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B46:E46"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A33:A45"/>
+    <mergeCell ref="A33:A49"/>
     <mergeCell ref="A14:A32"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B42:E42"/>
@@ -2208,17 +2296,6 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B33:E33"/>
-    <mergeCell ref="A46:A54"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1" display="ftp.baires.dc.fi.uba.ar"/>
@@ -2234,7 +2311,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2246,7 +2323,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalizado tabla de dns, agregue nuevos .rev que faltaban (falta verificar que funcione, los .rev con numeros no los toque, faltaria ver si hay que modificarlos)
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
+++ b/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="172">
   <si>
     <t>R1</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Enlaces</t>
   </si>
   <si>
-    <t>Raleigh - 10.47.2.0/24 - (.orbea.elcalafate.stacruz.dc.fi.uba.ar)</t>
-  </si>
-  <si>
     <t>hosta.trek6.rioturbio.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
@@ -465,12 +462,6 @@
     <t>r16.ghost2.stacruz.dc.fi.uba.ar</t>
   </si>
   <si>
-    <t>r2.orbea1.elcalafate.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
-    <t>r16.orbea2.elcalafate.stacruz.dc.fi.uba.ar</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -520,6 +511,27 @@
   </si>
   <si>
     <t>hostc.scott3.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r2.raleigh1.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r16.raleigh2.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>Raleigh - 10.47.2.0/24 - (.raleigh.elcalafate.stacruz.dc.fi.uba.ar)</t>
+  </si>
+  <si>
+    <t>MMR - 10.47.2.0/24 - (.mmr.elcalafate.stacruz.dc.fi.uba.ar)</t>
+  </si>
+  <si>
+    <t>.6</t>
+  </si>
+  <si>
+    <t>r11.mmr1.elcalafate.stacruz.dc.fi.uba.ar</t>
+  </si>
+  <si>
+    <t>r13.mmr2.elcalafate.stacruz.dc.fi.uba.ar</t>
   </si>
 </sst>
 </file>
@@ -609,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -803,6 +815,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -838,9 +863,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -925,9 +947,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -967,6 +986,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -976,15 +1004,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,6 +1011,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1300,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:D48"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1318,48 +1343,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>93</v>
+      <c r="E3" s="40" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1368,13 +1393,13 @@
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="42" t="s">
-        <v>94</v>
+      <c r="E4" s="40" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1383,13 +1408,13 @@
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="42" t="s">
-        <v>95</v>
+      <c r="E5" s="40" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1398,13 +1423,13 @@
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>96</v>
+      <c r="E6" s="40" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1414,51 +1439,51 @@
         <v>42</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>91</v>
+      <c r="E8" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56"/>
-      <c r="B9" s="52" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="41" t="s">
-        <v>152</v>
+      <c r="E10" s="39" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1467,13 +1492,13 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>155</v>
+      <c r="E11" s="39" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1482,54 +1507,54 @@
       <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>153</v>
+      <c r="E12" s="39" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="52"/>
+      <c r="B13" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>92</v>
+      <c r="E13" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="41" t="s">
-        <v>97</v>
+      <c r="E15" s="39" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1538,52 +1563,52 @@
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
-      <c r="B17" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="19" t="s">
+    <row r="18" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+    </row>
+    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="56"/>
-      <c r="B18" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="B19" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="51"/>
+      <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1592,13 +1617,13 @@
       <c r="D20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="41" t="s">
-        <v>101</v>
+      <c r="E20" s="39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1607,52 +1632,52 @@
       <c r="D21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="39" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56"/>
-      <c r="B22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
-      <c r="B23" s="52" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="28" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="43" t="s">
-        <v>158</v>
+      <c r="E24" s="41" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1661,13 +1686,13 @@
       <c r="D25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="41" t="s">
-        <v>104</v>
+      <c r="E25" s="39" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1676,13 +1701,13 @@
       <c r="D26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="41" t="s">
-        <v>105</v>
+      <c r="E26" s="39" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -1691,52 +1716,52 @@
       <c r="D27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="51"/>
+      <c r="B28" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="51"/>
+      <c r="B29" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="55"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="51"/>
+      <c r="B30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="39" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
-      <c r="B28" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56"/>
-      <c r="B29" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-    </row>
-    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="11" t="s">
+      <c r="A31" s="51"/>
+      <c r="B31" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1745,54 +1770,54 @@
       <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
-      <c r="B32" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="33" t="s">
+      <c r="A34" s="51"/>
+      <c r="B34" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="34" t="s">
-        <v>113</v>
+      <c r="E34" s="33" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1802,12 +1827,12 @@
         <v>45</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1816,52 +1841,52 @@
       <c r="D36" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="44" t="s">
-        <v>111</v>
+      <c r="E36" s="42" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="56"/>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="51"/>
+      <c r="B37" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="41" t="s">
-        <v>110</v>
+      <c r="E37" s="39" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="56"/>
-      <c r="B38" s="52" t="s">
+      <c r="A38" s="51"/>
+      <c r="B38" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
     </row>
     <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="33" t="s">
+      <c r="A39" s="51"/>
+      <c r="B39" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="34" t="s">
-        <v>116</v>
+      <c r="E39" s="33" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="51"/>
+      <c r="B40" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1871,378 +1896,378 @@
         <v>74</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="56"/>
-      <c r="B41" s="22" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="27" t="s">
-        <v>114</v>
+      <c r="E41" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56"/>
-      <c r="B42" s="52" t="s">
+      <c r="A42" s="51"/>
+      <c r="B42" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="56"/>
-      <c r="B43" s="35" t="s">
+      <c r="A43" s="51"/>
+      <c r="B43" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="37" t="s">
+      <c r="E43" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="55"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="51"/>
+      <c r="B45" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="56"/>
-      <c r="B44" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="54"/>
-    </row>
-    <row r="45" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="56"/>
-      <c r="B45" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E45" s="21" t="s">
+    <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="51"/>
+      <c r="B46" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="55"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="51"/>
+      <c r="B47" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="51"/>
+      <c r="B48" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="52"/>
+      <c r="B49" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="53" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56"/>
-      <c r="B46" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="54"/>
-    </row>
-    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="22" t="s">
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="55"/>
+    </row>
+    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="51"/>
+      <c r="B51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>161</v>
-      </c>
-      <c r="D47" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="56"/>
-      <c r="B48" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="D48" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="57"/>
-      <c r="B49" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="54"/>
-    </row>
-    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="51"/>
+      <c r="B52" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E52" s="42" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="56"/>
-      <c r="B52" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" s="45" t="s">
+    <row r="53" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="51"/>
+      <c r="B53" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="55"/>
+    </row>
+    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="51"/>
+      <c r="B54" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="51"/>
+      <c r="B55" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="51"/>
+      <c r="B56" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="55"/>
+    </row>
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="51"/>
+      <c r="B57" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="51"/>
+      <c r="B58" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="56"/>
-      <c r="B53" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="54"/>
-    </row>
-    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="56"/>
-      <c r="B55" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="56"/>
-      <c r="B56" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="54"/>
-    </row>
-    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="27" t="s">
+      <c r="E58" s="26" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="56"/>
-      <c r="B58" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="36" t="s">
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="52" t="s">
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="55"/>
+    </row>
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="51"/>
+      <c r="B60" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="54"/>
-    </row>
-    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="51"/>
+      <c r="B61" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="42" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="56"/>
-      <c r="B61" s="22" t="s">
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="51"/>
+      <c r="B62" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" s="54"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="55"/>
+    </row>
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="51"/>
+      <c r="B63" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="45" t="s">
+      <c r="C63" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D63" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="56"/>
-      <c r="B62" s="52" t="s">
+      <c r="E63" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="54"/>
-    </row>
-    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="50" t="s">
+    </row>
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="51"/>
+      <c r="B64" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="D63" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="42" t="s">
+      <c r="D64" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="40" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="56"/>
-      <c r="B64" s="22" t="s">
+    <row r="65" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="51"/>
+      <c r="B65" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="54"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="55"/>
+    </row>
+    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="51"/>
+      <c r="B66" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="51"/>
+      <c r="B67" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="D64" s="25" t="s">
+      <c r="C67" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E64" s="42" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="56"/>
-      <c r="B65" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="54"/>
-    </row>
-    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56"/>
-      <c r="B66" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="27" t="s">
+      <c r="E67" s="26" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="56"/>
-      <c r="B67" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C67" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E67" s="27" t="s">
-        <v>148</v>
-      </c>
-    </row>
     <row r="68" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="55" t="s">
+      <c r="A68" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="B68" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="54"/>
+      <c r="B68" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="55"/>
     </row>
     <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="56"/>
-      <c r="B69" s="11" t="s">
+      <c r="A69" s="51"/>
+      <c r="B69" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2251,39 +2276,68 @@
       <c r="D69" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E69" s="38" t="s">
-        <v>149</v>
+      <c r="E69" s="60" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="57"/>
-      <c r="B70" s="39" t="s">
+      <c r="A70" s="51"/>
+      <c r="B70" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="51" t="s">
+      <c r="C70" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="38" t="s">
-        <v>150</v>
+      <c r="E70" s="60" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="51"/>
+      <c r="B71" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="55"/>
+    </row>
+    <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="51"/>
+      <c r="B72" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="52"/>
+      <c r="B73" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" s="60" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="A50:A58"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B46:E46"/>
+  <mergeCells count="25">
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="A68:A73"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A33:A49"/>
@@ -2296,6 +2350,17 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B33:E33"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B65:E65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1" display="ftp.baires.dc.fi.uba.ar"/>

</xml_diff>

<commit_message>
Correccion de mal formateo de tabla dns
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
+++ b/ tp-distribuidos-grupo3/DNS/dns.hostnames.xlsx
@@ -897,11 +897,11 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1029,29 +1029,26 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1428,7 +1425,7 @@
   <dimension ref="A1:AMK73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,29 +1440,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
@@ -1559,12 +1556,12 @@
     </row>
     <row r="9" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46"/>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
@@ -1627,15 +1624,15 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
     </row>
     <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
@@ -1684,12 +1681,12 @@
     </row>
     <row r="18" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="46"/>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
     </row>
     <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
@@ -1753,12 +1750,12 @@
     </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="46"/>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
@@ -1837,12 +1834,12 @@
     </row>
     <row r="29" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="46"/>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
     </row>
     <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="46"/>
@@ -1875,7 +1872,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="27" t="s">
         <v>75</v>
       </c>
@@ -1890,15 +1887,15 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
@@ -1962,12 +1959,12 @@
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="46"/>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
     </row>
     <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
@@ -2016,12 +2013,12 @@
     </row>
     <row r="42" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="46"/>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
     </row>
     <row r="43" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="46"/>
@@ -2040,12 +2037,12 @@
     </row>
     <row r="44" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="46"/>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
     </row>
     <row r="45" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="46"/>
@@ -2064,12 +2061,12 @@
     </row>
     <row r="46" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="46"/>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
     </row>
     <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="46"/>
@@ -2102,7 +2099,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="47"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="36" t="s">
         <v>127</v>
       </c>
@@ -2117,18 +2114,18 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
     </row>
     <row r="51" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="44"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="23" t="s">
         <v>6</v>
       </c>
@@ -2143,7 +2140,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="44"/>
+      <c r="A52" s="49"/>
       <c r="B52" s="27" t="s">
         <v>122</v>
       </c>
@@ -2158,16 +2155,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="44"/>
-      <c r="B53" s="43" t="s">
+      <c r="A53" s="49"/>
+      <c r="B53" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
     </row>
     <row r="54" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="44"/>
+      <c r="A54" s="49"/>
       <c r="B54" s="26" t="s">
         <v>6</v>
       </c>
@@ -2182,7 +2179,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="44"/>
+      <c r="A55" s="49"/>
       <c r="B55" s="27" t="s">
         <v>78</v>
       </c>
@@ -2197,16 +2194,16 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="44"/>
-      <c r="B56" s="43" t="s">
+      <c r="A56" s="49"/>
+      <c r="B56" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
     </row>
     <row r="57" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="44"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="27" t="s">
         <v>78</v>
       </c>
@@ -2221,7 +2218,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="44"/>
+      <c r="A58" s="49"/>
       <c r="B58" s="14" t="s">
         <v>122</v>
       </c>
@@ -2236,18 +2233,18 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
     </row>
     <row r="60" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="44"/>
+      <c r="A60" s="49"/>
       <c r="B60" s="23" t="s">
         <v>33</v>
       </c>
@@ -2262,7 +2259,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="44"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="27" t="s">
         <v>56</v>
       </c>
@@ -2277,16 +2274,16 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="44"/>
-      <c r="B62" s="43" t="s">
+      <c r="A62" s="49"/>
+      <c r="B62" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
     </row>
     <row r="63" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="44"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="23" t="s">
         <v>56</v>
       </c>
@@ -2301,7 +2298,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="44"/>
+      <c r="A64" s="49"/>
       <c r="B64" s="27" t="s">
         <v>104</v>
       </c>
@@ -2316,16 +2313,16 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="44"/>
-      <c r="B65" s="43" t="s">
+      <c r="A65" s="49"/>
+      <c r="B65" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="44"/>
+      <c r="A66" s="49"/>
       <c r="B66" s="17" t="s">
         <v>33</v>
       </c>
@@ -2340,7 +2337,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="44"/>
+      <c r="A67" s="49"/>
       <c r="B67" s="32" t="s">
         <v>104</v>
       </c>
@@ -2355,15 +2352,15 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
     </row>
     <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="46"/>
@@ -2397,12 +2394,12 @@
     </row>
     <row r="71" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="46"/>
-      <c r="B71" s="43" t="s">
+      <c r="B71" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
     </row>
     <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="46"/>
@@ -2420,7 +2417,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="47"/>
+      <c r="A73" s="48"/>
       <c r="B73" s="14" t="s">
         <v>122</v>
       </c>
@@ -2436,20 +2433,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="A14:A32"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="A33:A49"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B46:E46"/>
     <mergeCell ref="A68:A73"/>
     <mergeCell ref="B68:E68"/>
     <mergeCell ref="B71:E71"/>
@@ -2461,6 +2444,20 @@
     <mergeCell ref="B59:E59"/>
     <mergeCell ref="B62:E62"/>
     <mergeCell ref="B65:E65"/>
+    <mergeCell ref="A33:A49"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A14:A32"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>